<commit_message>
Natively plotted thermophysical props, added fracture toughness, and added 1_3 models and plots files
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\F82H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GhoniemDesktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4189030B-D063-4CC4-BD80-13674C083519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CAB848-777F-4A05-9B9A-F1E9F3084D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="614" activeTab="2" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="720" yWindow="2780" windowWidth="25400" windowHeight="15360" tabRatio="736" firstSheet="6" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diffusivity" sheetId="2" r:id="rId1"/>
-    <sheet name="Yield Strength" sheetId="7" r:id="rId2"/>
-    <sheet name="Ultimate Strength" sheetId="6" r:id="rId3"/>
-    <sheet name="Uniform Elongation" sheetId="9" r:id="rId4"/>
-    <sheet name="Total Elongation" sheetId="10" r:id="rId5"/>
-    <sheet name="HT-9 Creep Strain" sheetId="12" r:id="rId6"/>
-    <sheet name="T91 Creep Strain" sheetId="13" r:id="rId7"/>
-    <sheet name="F82H Creep Strain" sheetId="14" r:id="rId8"/>
-    <sheet name="Fatigue" sheetId="15" r:id="rId9"/>
+    <sheet name="Contents" sheetId="2" r:id="rId1"/>
+    <sheet name="Thermal Emissivity" sheetId="16" r:id="rId2"/>
+    <sheet name="Yield Strength" sheetId="7" r:id="rId3"/>
+    <sheet name="Ultimate Strength" sheetId="6" r:id="rId4"/>
+    <sheet name="Uniform Elongation" sheetId="9" r:id="rId5"/>
+    <sheet name="Total Elongation" sheetId="10" r:id="rId6"/>
+    <sheet name="HT-9 Creep Strain" sheetId="12" r:id="rId7"/>
+    <sheet name="T91 Creep Strain" sheetId="13" r:id="rId8"/>
+    <sheet name="F82H Creep Strain" sheetId="14" r:id="rId9"/>
+    <sheet name="Fatigue" sheetId="15" r:id="rId10"/>
+    <sheet name="Toughness" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,11 +46,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
   <si>
     <t>F82H</t>
   </si>
   <si>
+    <t>Property of Interest</t>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>Associated References</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
     <t>CEA_u</t>
   </si>
   <si>
@@ -229,6 +243,27 @@
     <t>log10(Strain amplitude)_H_T673</t>
   </si>
   <si>
+    <t>Yield Strength</t>
+  </si>
+  <si>
+    <t>Ultimate Strength</t>
+  </si>
+  <si>
+    <t>Uniform Elongation</t>
+  </si>
+  <si>
+    <t>Total Elongation</t>
+  </si>
+  <si>
+    <t>HT-9 Creep Strain</t>
+  </si>
+  <si>
+    <t>T91 Creep Strain</t>
+  </si>
+  <si>
+    <t>F82H Creep Strain</t>
+  </si>
+  <si>
     <t>Tavassoli_y (MPa)</t>
   </si>
   <si>
@@ -283,66 +318,30 @@
     <t>T_JAERI_t (C)</t>
   </si>
   <si>
-    <t>EUROFER97-Mergia</t>
-  </si>
-  <si>
-    <t>Temp (K)</t>
-  </si>
-  <si>
-    <r>
-      <t>Thermal Diffusivity Coef. (cm</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/s)</t>
-    </r>
-  </si>
-  <si>
-    <t>Reference: Figure 3 Mergia, K., and N. Boukos. "Structural, thermal, electrical and magnetic properties of Eurofer 97 steel." Journal of Nuclear Materials 373.1-3 (2008): 1-8.</t>
-  </si>
-  <si>
-    <t>Mergia&amp;Boukos</t>
+    <t>polished_sigma</t>
+  </si>
+  <si>
+    <t>rolled_sigma</t>
+  </si>
+  <si>
+    <t>T_polished_sigma (K)</t>
+  </si>
+  <si>
+    <t>T_rolled_sigma (K)</t>
+  </si>
+  <si>
+    <t>T_IEA_K (T)</t>
+  </si>
+  <si>
+    <t>IEA_K [MPa m^(1/2)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -367,11 +366,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,29 +381,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,61 +404,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142019</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>86863</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB7C148-AC88-41E1-A9A2-113A0EE0CEF5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3850419"/>
-          <a:ext cx="3549650" cy="2707094"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -631,7 +558,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -786,7 +713,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -991,7 +918,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1146,7 +1073,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1201,7 +1128,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1256,7 +1183,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1311,7 +1238,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1405,6 +1332,55 @@
         <a:xfrm>
           <a:off x="4870450" y="2667000"/>
           <a:ext cx="7772400" cy="7020232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>324904</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>89373</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81D5365C-AAFF-48FE-862D-146BF1A80FD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2787650" y="146050"/>
+          <a:ext cx="6312954" cy="5099523"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1733,68 +1709,819 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27109A3A-4496-48FB-9A48-4CA7AFC9B114}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="77.6328125" customWidth="1"/>
+    <col min="4" max="4" width="59.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E579750B-800F-40F2-8460-1ADC1CC14203}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="4" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="4"/>
+    <col min="1" max="1" width="21.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="45.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="9"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="7" t="s">
-        <v>83</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>3.2871329080508902</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-0.60479502036177002</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3.2889151934788501</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-0.83658124026889003</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.2994609427281101</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-0.40805593013441099</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.02874588718245</v>
+      </c>
+      <c r="H3" s="3">
+        <v>-1.9901911235340799</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4.0424718810385896</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-2.2075029169747999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3.4270419687890001</v>
+      </c>
+      <c r="L3" s="3">
+        <v>-1.98422534630182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>3.6013061125664598</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-0.66302026761183797</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.60439989104519</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-1.0653661587713701</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3.5863214637607599</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-0.51426669043047302</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3.0748816436830202</v>
+      </c>
+      <c r="H4" s="3">
+        <v>-1.8195187358823299</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4.1219445239038102</v>
+      </c>
+      <c r="J4" s="3">
+        <v>-2.21301532735083</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3.4846265716378002</v>
+      </c>
+      <c r="L4" s="3">
+        <v>-1.9785772487700199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>3.8966543475994602</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-0.67305823365425699</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.9086057483749301</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-1.0273379045031299</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.9136297756001799</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-0.48071264514697098</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.9908409229214201</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-1.8167998927315301</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3.67777170381525</v>
+      </c>
+      <c r="L5" s="3">
+        <v>-2.1182572999288301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>4.2010619730908498</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-0.661269928809467</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.9097827293179201</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-1.1804042761399101</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.90965494281554</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-0.56378564150505595</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.53212381256898</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-2.0848266685920001</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3.7663610202881799</v>
+      </c>
+      <c r="L6" s="3">
+        <v>-2.1097830907759398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>4.5059740189863797</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-0.71508149752329597</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.2019295761859796</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-1.37410171133029</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4.2097850832798098</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-0.59571040888318005</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.7165740100873599</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-2.2105288129299798</v>
+      </c>
+      <c r="K7" s="3">
+        <v>4.3218466679731398</v>
+      </c>
+      <c r="L7" s="3">
+        <v>-2.2938805400554898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>4.8105161565855399</v>
+      </c>
+      <c r="B8" s="3">
+        <v>-0.72078649229413805</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4.51323767280602</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-1.6597196767674001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.5100497358518501</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-0.645128475876934</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.8684723525832099</v>
+      </c>
+      <c r="H8" s="3">
+        <v>-2.07891865130527</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4.3838560952214003</v>
+      </c>
+      <c r="L8" s="3">
+        <v>-2.2882283168133002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>5.4107091814602004</v>
+      </c>
+      <c r="B9" s="3">
+        <v>-0.77588937724256901</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.8180152065937802</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-1.6960379458656001</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4.8103480164508303</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-0.69891986777459802</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3.9871071550132502</v>
+      </c>
+      <c r="H9" s="3">
+        <v>-2.1543325116293501</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4.6482006745536504</v>
+      </c>
+      <c r="L9" s="3">
+        <v>-2.3914783451775601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>5.7111419741669502</v>
+      </c>
+      <c r="B10" s="3">
+        <v>-0.84717406875586398</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5.4240595081564802</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-2.5120993640940101</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.4198694559994101</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-0.76718308106708399</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4.0042185388796598</v>
+      </c>
+      <c r="H10" s="3">
+        <v>-2.2074634101059298</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4.7412457582540002</v>
+      </c>
+      <c r="L10" s="3">
+        <v>-2.3802027786659501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
+        <v>5.7114917056471599</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-2.6926566477565101</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5.7248151299218799</v>
+      </c>
+      <c r="F11" s="3">
+        <v>-0.82536797468482104</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4.6361329716460604</v>
+      </c>
+      <c r="H11" s="3">
+        <v>-2.2823986880240899</v>
+      </c>
+      <c r="K11" s="3">
+        <v>4.85567233608037</v>
+      </c>
+      <c r="L11" s="3">
+        <v>-2.4360401431621499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G12" s="3">
+        <v>4.4800264045465301</v>
+      </c>
+      <c r="H12" s="3">
+        <v>-2.3944323538209198</v>
+      </c>
+      <c r="K12" s="3">
+        <v>5.0902189720792599</v>
+      </c>
+      <c r="L12" s="3">
+        <v>-2.43302424886285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G13" s="3">
+        <v>4.6436830216702996</v>
+      </c>
+      <c r="H13" s="3">
+        <v>-2.3998741658329301</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5.1695873258176697</v>
+      </c>
+      <c r="L13" s="3">
+        <v>-2.4581250709106501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K14" s="3">
+        <v>5.6121316514187303</v>
+      </c>
+      <c r="L14" s="3">
+        <v>-2.45211803657442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K15" s="3">
+        <v>5.91308159623736</v>
+      </c>
+      <c r="L15" s="3">
+        <v>-2.44624302497086</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K16" s="3">
+        <v>6.0370385650779301</v>
+      </c>
+      <c r="L16" s="3">
+        <v>-2.4405330417831301</v>
+      </c>
+    </row>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K17" s="3">
+        <v>6.0989242210143102</v>
+      </c>
+      <c r="L17" s="3">
+        <v>-2.4460697451342401</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA6CA63-0F6B-4003-854E-C3B2C624AC7C}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>-160.54564529999999</v>
+      </c>
+      <c r="B3">
+        <v>48.627568109999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>-160.1259182</v>
+      </c>
+      <c r="B4">
+        <v>38.015177770000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-160.1259182</v>
+      </c>
+      <c r="B5">
+        <v>30.524541070000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B6">
+        <v>65.387179979999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B7">
+        <v>76.623135039999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B8">
+        <v>97.222385970000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B9">
+        <v>110.33100020000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B10">
+        <v>130.93025109999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-100.1049318</v>
+      </c>
+      <c r="B11">
+        <v>178.3709503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-49.737670510000001</v>
+      </c>
+      <c r="B12">
+        <v>97.768005099999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>-49.737670510000001</v>
+      </c>
+      <c r="B13">
+        <v>246.95651950000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>-50.157397690000003</v>
+      </c>
+      <c r="B14">
+        <v>260.06578869999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>-49.737670510000001</v>
+      </c>
+      <c r="B15">
+        <v>275.04640710000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>-50.157397690000003</v>
+      </c>
+      <c r="B16">
+        <v>290.02833550000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>-50.157397690000003</v>
+      </c>
+      <c r="B17">
+        <v>318.74244290000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>-19.937040920000001</v>
+      </c>
+      <c r="B18">
+        <v>279.9936596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>-19.937040920000001</v>
+      </c>
+      <c r="B19">
+        <v>333.05233620000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A36:B36"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A38" r:id="rId1" xr:uid="{7A4F8865-921F-4EF1-98AE-7028C0CEC4B4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2966564E-4C1C-4AED-858E-DA4E71B509BC}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>429.17127071823199</v>
+      </c>
+      <c r="B3">
+        <v>0.11873198847262199</v>
+      </c>
+      <c r="C3">
+        <v>471.71270718232</v>
+      </c>
+      <c r="D3">
+        <v>0.18141210374639699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>524.30939226519297</v>
+      </c>
+      <c r="B4">
+        <v>0.129971181556195</v>
+      </c>
+      <c r="C4">
+        <v>573.03867403314905</v>
+      </c>
+      <c r="D4">
+        <v>0.21512968299711799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>626.40883977900501</v>
+      </c>
+      <c r="B5">
+        <v>0.14293948126801101</v>
+      </c>
+      <c r="C5">
+        <v>673.59116022099397</v>
+      </c>
+      <c r="D5">
+        <v>0.244524495677233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>726.96132596685004</v>
+      </c>
+      <c r="B6">
+        <v>0.15547550432276599</v>
+      </c>
+      <c r="C6">
+        <v>772.596685082872</v>
+      </c>
+      <c r="D6">
+        <v>0.27391930835734801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>822.87292817679497</v>
+      </c>
+      <c r="B7">
+        <v>0.17449567723342899</v>
+      </c>
+      <c r="C7">
+        <v>874.69613259668495</v>
+      </c>
+      <c r="D7">
+        <v>0.30244956772334203</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D931B76-7C5F-495B-8FF4-78E0CE47C1ED}">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -1813,57 +2540,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -2189,11 +2916,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61307E5D-2D7B-4CE3-B2DB-16307B2B26EE}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -2212,49 +2939,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2544,7 +3271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41CB5B8-2BC3-43D2-A2E9-D01F45547500}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -2560,41 +3287,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2832,7 +3559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2DAEC4-8637-41BC-BD00-C4174E60E61C}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -2848,49 +3575,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -3150,7 +3877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DD7C9E-CEDE-49A6-8629-4EA5CF8E31A8}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3171,41 +3898,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -3439,7 +4166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506D56C3-70C9-43BD-850D-D9A3393EFBBB}">
   <dimension ref="A1:P58"/>
   <sheetViews>
@@ -3468,73 +4195,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -5752,7 +6479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8CD3D0-7518-4827-989C-484F0B819C0C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -5770,25 +6497,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -6144,446 +6871,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E579750B-800F-40F2-8460-1ADC1CC14203}">
-  <dimension ref="A1:L17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>3.2871329080508902</v>
-      </c>
-      <c r="B3" s="3">
-        <v>-0.60479502036177002</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3.2889151934788501</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-0.83658124026889003</v>
-      </c>
-      <c r="E3" s="3">
-        <v>3.2994609427281101</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-0.40805593013441099</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3.02874588718245</v>
-      </c>
-      <c r="H3" s="3">
-        <v>-1.9901911235340799</v>
-      </c>
-      <c r="I3" s="3">
-        <v>4.0424718810385896</v>
-      </c>
-      <c r="J3" s="3">
-        <v>-2.2075029169747999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3.4270419687890001</v>
-      </c>
-      <c r="L3" s="3">
-        <v>-1.98422534630182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3.6013061125664598</v>
-      </c>
-      <c r="B4" s="3">
-        <v>-0.66302026761183797</v>
-      </c>
-      <c r="C4" s="3">
-        <v>3.60439989104519</v>
-      </c>
-      <c r="D4" s="3">
-        <v>-1.0653661587713701</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3.5863214637607599</v>
-      </c>
-      <c r="F4" s="3">
-        <v>-0.51426669043047302</v>
-      </c>
-      <c r="G4" s="3">
-        <v>3.0748816436830202</v>
-      </c>
-      <c r="H4" s="3">
-        <v>-1.8195187358823299</v>
-      </c>
-      <c r="I4" s="3">
-        <v>4.1219445239038102</v>
-      </c>
-      <c r="J4" s="3">
-        <v>-2.21301532735083</v>
-      </c>
-      <c r="K4" s="3">
-        <v>3.4846265716378002</v>
-      </c>
-      <c r="L4" s="3">
-        <v>-1.9785772487700199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>3.8966543475994602</v>
-      </c>
-      <c r="B5" s="3">
-        <v>-0.67305823365425699</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3.9086057483749301</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-1.0273379045031299</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3.9136297756001799</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-0.48071264514697098</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2.9908409229214201</v>
-      </c>
-      <c r="H5" s="3">
-        <v>-1.8167998927315301</v>
-      </c>
-      <c r="K5" s="3">
-        <v>3.67777170381525</v>
-      </c>
-      <c r="L5" s="3">
-        <v>-2.1182572999288301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>4.2010619730908498</v>
-      </c>
-      <c r="B6" s="3">
-        <v>-0.661269928809467</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3.9097827293179201</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-1.1804042761399101</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.90965494281554</v>
-      </c>
-      <c r="F6" s="3">
-        <v>-0.56378564150505595</v>
-      </c>
-      <c r="G6" s="3">
-        <v>3.53212381256898</v>
-      </c>
-      <c r="H6" s="3">
-        <v>-2.0848266685920001</v>
-      </c>
-      <c r="K6" s="3">
-        <v>3.7663610202881799</v>
-      </c>
-      <c r="L6" s="3">
-        <v>-2.1097830907759398</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>4.5059740189863797</v>
-      </c>
-      <c r="B7" s="3">
-        <v>-0.71508149752329597</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4.2019295761859796</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-1.37410171133029</v>
-      </c>
-      <c r="E7" s="3">
-        <v>4.2097850832798098</v>
-      </c>
-      <c r="F7" s="3">
-        <v>-0.59571040888318005</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3.7165740100873599</v>
-      </c>
-      <c r="H7" s="3">
-        <v>-2.2105288129299798</v>
-      </c>
-      <c r="K7" s="3">
-        <v>4.3218466679731398</v>
-      </c>
-      <c r="L7" s="3">
-        <v>-2.2938805400554898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>4.8105161565855399</v>
-      </c>
-      <c r="B8" s="3">
-        <v>-0.72078649229413805</v>
-      </c>
-      <c r="C8" s="3">
-        <v>4.51323767280602</v>
-      </c>
-      <c r="D8" s="3">
-        <v>-1.6597196767674001</v>
-      </c>
-      <c r="E8" s="3">
-        <v>4.5100497358518501</v>
-      </c>
-      <c r="F8" s="3">
-        <v>-0.645128475876934</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3.8684723525832099</v>
-      </c>
-      <c r="H8" s="3">
-        <v>-2.07891865130527</v>
-      </c>
-      <c r="K8" s="3">
-        <v>4.3838560952214003</v>
-      </c>
-      <c r="L8" s="3">
-        <v>-2.2882283168133002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>5.4107091814602004</v>
-      </c>
-      <c r="B9" s="3">
-        <v>-0.77588937724256901</v>
-      </c>
-      <c r="C9" s="3">
-        <v>4.8180152065937802</v>
-      </c>
-      <c r="D9" s="3">
-        <v>-1.6960379458656001</v>
-      </c>
-      <c r="E9" s="3">
-        <v>4.8103480164508303</v>
-      </c>
-      <c r="F9" s="3">
-        <v>-0.69891986777459802</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3.9871071550132502</v>
-      </c>
-      <c r="H9" s="3">
-        <v>-2.1543325116293501</v>
-      </c>
-      <c r="K9" s="3">
-        <v>4.6482006745536504</v>
-      </c>
-      <c r="L9" s="3">
-        <v>-2.3914783451775601</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>5.7111419741669502</v>
-      </c>
-      <c r="B10" s="3">
-        <v>-0.84717406875586398</v>
-      </c>
-      <c r="C10" s="3">
-        <v>5.4240595081564802</v>
-      </c>
-      <c r="D10" s="3">
-        <v>-2.5120993640940101</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5.4198694559994101</v>
-      </c>
-      <c r="F10" s="3">
-        <v>-0.76718308106708399</v>
-      </c>
-      <c r="G10" s="3">
-        <v>4.0042185388796598</v>
-      </c>
-      <c r="H10" s="3">
-        <v>-2.2074634101059298</v>
-      </c>
-      <c r="K10" s="3">
-        <v>4.7412457582540002</v>
-      </c>
-      <c r="L10" s="3">
-        <v>-2.3802027786659501</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C11" s="3">
-        <v>5.7114917056471599</v>
-      </c>
-      <c r="D11" s="3">
-        <v>-2.6926566477565101</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5.7248151299218799</v>
-      </c>
-      <c r="F11" s="3">
-        <v>-0.82536797468482104</v>
-      </c>
-      <c r="G11" s="3">
-        <v>4.6361329716460604</v>
-      </c>
-      <c r="H11" s="3">
-        <v>-2.2823986880240899</v>
-      </c>
-      <c r="K11" s="3">
-        <v>4.85567233608037</v>
-      </c>
-      <c r="L11" s="3">
-        <v>-2.4360401431621499</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G12" s="3">
-        <v>4.4800264045465301</v>
-      </c>
-      <c r="H12" s="3">
-        <v>-2.3944323538209198</v>
-      </c>
-      <c r="K12" s="3">
-        <v>5.0902189720792599</v>
-      </c>
-      <c r="L12" s="3">
-        <v>-2.43302424886285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G13" s="3">
-        <v>4.6436830216702996</v>
-      </c>
-      <c r="H13" s="3">
-        <v>-2.3998741658329301</v>
-      </c>
-      <c r="K13" s="3">
-        <v>5.1695873258176697</v>
-      </c>
-      <c r="L13" s="3">
-        <v>-2.4581250709106501</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="K14" s="3">
-        <v>5.6121316514187303</v>
-      </c>
-      <c r="L14" s="3">
-        <v>-2.45211803657442</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="K15" s="3">
-        <v>5.91308159623736</v>
-      </c>
-      <c r="L15" s="3">
-        <v>-2.44624302497086</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="K16" s="3">
-        <v>6.0370385650779301</v>
-      </c>
-      <c r="L16" s="3">
-        <v>-2.4405330417831301</v>
-      </c>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K17" s="3">
-        <v>6.0989242210143102</v>
-      </c>
-      <c r="L17" s="3">
-        <v>-2.4460697451342401</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added many GDrive citations; added Hardness data+cell
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GhoniemDesktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GhoniemDesktop\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CAB848-777F-4A05-9B9A-F1E9F3084D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89408A-A03D-4B3A-8925-DA59DD9AA204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2780" windowWidth="25400" windowHeight="15360" tabRatio="736" firstSheet="6" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="2660" yWindow="3460" windowWidth="17470" windowHeight="16010" tabRatio="736" firstSheet="6" activeTab="11" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="F82H Creep Strain" sheetId="14" r:id="rId9"/>
     <sheet name="Fatigue" sheetId="15" r:id="rId10"/>
     <sheet name="Toughness" sheetId="17" r:id="rId11"/>
+    <sheet name="Hardness" sheetId="18" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>F82H</t>
   </si>
@@ -330,10 +331,22 @@
     <t>T_rolled_sigma (K)</t>
   </si>
   <si>
-    <t>T_IEA_K (T)</t>
-  </si>
-  <si>
-    <t>IEA_K [MPa m^(1/2)]</t>
+    <t>Vickers</t>
+  </si>
+  <si>
+    <t>T_microindentation (K)</t>
+  </si>
+  <si>
+    <t>microindentation (GPa)</t>
+  </si>
+  <si>
+    <t>T_Vickers (K)</t>
+  </si>
+  <si>
+    <t>T_IEA (C)</t>
+  </si>
+  <si>
+    <t>IEA [MPa m^(1/2)]</t>
   </si>
 </sst>
 </file>
@@ -551,6 +564,72 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>127078</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>170961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>77944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{608CD508-7916-A1DF-199B-589AC8DC5B38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3893116" y="170961"/>
+          <a:ext cx="2932507" cy="5475445"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2236,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA6CA63-0F6B-4003-854E-C3B2C624AC7C}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2254,10 +2333,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2399,6 +2478,130 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E880377-A00F-4DE4-8CA1-38FE84BDA18D}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>971.678504538065</v>
+      </c>
+      <c r="B3">
+        <v>4.4167497507477496</v>
+      </c>
+      <c r="C3">
+        <v>1022.67345251068</v>
+      </c>
+      <c r="D3">
+        <v>200.59820538384801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>991.07123075218703</v>
+      </c>
+      <c r="B4">
+        <v>4.2173479561315999</v>
+      </c>
+      <c r="C4">
+        <v>1073.10291348177</v>
+      </c>
+      <c r="D4">
+        <v>174.67597208374801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1022.1079655091499</v>
+      </c>
+      <c r="B5">
+        <v>3.7686939182452601</v>
+      </c>
+      <c r="C5">
+        <v>1083.44076298237</v>
+      </c>
+      <c r="D5">
+        <v>173.47956131605099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1051.8494902888201</v>
+      </c>
+      <c r="B6">
+        <v>3.3698903290129598</v>
+      </c>
+      <c r="C6">
+        <v>1090.55057051069</v>
+      </c>
+      <c r="D6">
+        <v>171.08673978065801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1073.1679638088301</v>
+      </c>
+      <c r="B7">
+        <v>3.3599202392821499</v>
+      </c>
+      <c r="C7">
+        <v>1112.4544969741901</v>
+      </c>
+      <c r="D7">
+        <v>208.17547357926199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>1151.56520103771</v>
+      </c>
+      <c r="D8">
+        <v>390.82751744765699</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2409,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2966564E-4C1C-4AED-858E-DA4E71B509BC}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4170,7 +4373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506D56C3-70C9-43BD-850D-D9A3393EFBBB}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reverted to old commit and then committed up-to-date downloaded ZIP of repo WITHOUT "Icon?" files
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GhoniemDesktop\F82H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89408A-A03D-4B3A-8925-DA59DD9AA204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDBA03-8FFF-4596-9150-9C1DA2CD6DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="3460" windowWidth="17470" windowHeight="16010" tabRatio="736" firstSheet="6" activeTab="11" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="17330" yWindow="4040" windowWidth="18500" windowHeight="16010" tabRatio="736" firstSheet="13" activeTab="14" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,9 @@
     <sheet name="Fatigue" sheetId="15" r:id="rId10"/>
     <sheet name="Toughness" sheetId="17" r:id="rId11"/>
     <sheet name="Hardness" sheetId="18" r:id="rId12"/>
+    <sheet name="Radiation Hardening 3D" sheetId="19" r:id="rId13"/>
+    <sheet name="Radiation Hardening - No Helium" sheetId="20" r:id="rId14"/>
+    <sheet name="Helium Hardening" sheetId="21" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
   <si>
     <t>F82H</t>
   </si>
@@ -347,6 +350,21 @@
   </si>
   <si>
     <t>IEA [MPa m^(1/2)]</t>
+  </si>
+  <si>
+    <t>T (K)</t>
+  </si>
+  <si>
+    <t>Dose (dpa)</t>
+  </si>
+  <si>
+    <t>delta_sigma_y (MPa)</t>
+  </si>
+  <si>
+    <t>delta_sigma_He (MPa)</t>
+  </si>
+  <si>
+    <t>He conc (appm)</t>
   </si>
 </sst>
 </file>
@@ -2488,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E880377-A00F-4DE4-8CA1-38FE84BDA18D}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2605,6 +2623,1782 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C0EEDE-2AC2-4AD2-B716-5AB199341C15}">
+  <dimension ref="A1:C119"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>523</v>
+      </c>
+      <c r="B3">
+        <v>26.921692201765943</v>
+      </c>
+      <c r="C3">
+        <v>645.01969245533905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>523</v>
+      </c>
+      <c r="B4">
+        <v>0.75293273217479795</v>
+      </c>
+      <c r="C4">
+        <v>111.033678174138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>523</v>
+      </c>
+      <c r="B5">
+        <v>0.75193592542110033</v>
+      </c>
+      <c r="C5">
+        <v>192.13807661628601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>523</v>
+      </c>
+      <c r="B6">
+        <v>0.94247961999210561</v>
+      </c>
+      <c r="C6">
+        <v>199.59627829121101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>523</v>
+      </c>
+      <c r="B7">
+        <v>0.7158800234842444</v>
+      </c>
+      <c r="C7">
+        <v>234.567587437665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>523</v>
+      </c>
+      <c r="B8">
+        <v>1.9792900552257218</v>
+      </c>
+      <c r="C8">
+        <v>140.83245505630899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>523</v>
+      </c>
+      <c r="B9">
+        <v>1.8648249361693843</v>
+      </c>
+      <c r="C9">
+        <v>112.145318880058</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>523</v>
+      </c>
+      <c r="B10">
+        <v>2.5345022167617204</v>
+      </c>
+      <c r="C10">
+        <v>361.63492608786601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>523</v>
+      </c>
+      <c r="B11">
+        <v>2.7018576502292566</v>
+      </c>
+      <c r="C11">
+        <v>381.58490661375902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>523</v>
+      </c>
+      <c r="B12">
+        <v>4.5451910213346922</v>
+      </c>
+      <c r="C12">
+        <v>281.63082507912901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>523</v>
+      </c>
+      <c r="B13">
+        <v>4.5466610951009665</v>
+      </c>
+      <c r="C13">
+        <v>232.96818601384001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>523</v>
+      </c>
+      <c r="B14">
+        <v>5.5703829520770247</v>
+      </c>
+      <c r="C14">
+        <v>277.825157152229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>523</v>
+      </c>
+      <c r="B15">
+        <v>7.3046587172369675</v>
+      </c>
+      <c r="C15">
+        <v>241.54653584906799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>523</v>
+      </c>
+      <c r="B16">
+        <v>7.7000973822121077</v>
+      </c>
+      <c r="C16">
+        <v>300.17140399572997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>523</v>
+      </c>
+      <c r="B17">
+        <v>9.8448975011591848</v>
+      </c>
+      <c r="C17">
+        <v>340.00046959433001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>523</v>
+      </c>
+      <c r="B18">
+        <v>8.9558297458649889</v>
+      </c>
+      <c r="C18">
+        <v>313.83721155141899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>523</v>
+      </c>
+      <c r="B19">
+        <v>9.9769605517523523</v>
+      </c>
+      <c r="C19">
+        <v>307.55303858121601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>523</v>
+      </c>
+      <c r="B20">
+        <v>9.081862195426293</v>
+      </c>
+      <c r="C20">
+        <v>280.14202056227202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>523</v>
+      </c>
+      <c r="B21">
+        <v>7.2967290770712099</v>
+      </c>
+      <c r="C21">
+        <v>448.674691870554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>523</v>
+      </c>
+      <c r="B22">
+        <v>20.12234918720829</v>
+      </c>
+      <c r="C22">
+        <v>379.560132470832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>523</v>
+      </c>
+      <c r="B23">
+        <v>26.62445208642394</v>
+      </c>
+      <c r="C23">
+        <v>395.59668398098398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>523</v>
+      </c>
+      <c r="B24">
+        <v>15.830912770717473</v>
+      </c>
+      <c r="C24">
+        <v>201.269410986346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>523</v>
+      </c>
+      <c r="B25">
+        <v>2.3466597209021121</v>
+      </c>
+      <c r="C25">
+        <v>64.685066700765205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>573</v>
+      </c>
+      <c r="B26">
+        <v>7.9055447548994379E-2</v>
+      </c>
+      <c r="C26">
+        <v>47.4193542695647</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>573</v>
+      </c>
+      <c r="B27">
+        <v>4.2852950339358896E-2</v>
+      </c>
+      <c r="C27">
+        <v>100.692819239323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>573</v>
+      </c>
+      <c r="B28">
+        <v>0.86942632347504101</v>
+      </c>
+      <c r="C28">
+        <v>113.80778748664299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>573</v>
+      </c>
+      <c r="B29">
+        <v>0.9871582050033012</v>
+      </c>
+      <c r="C29">
+        <v>164.08575471008899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>573</v>
+      </c>
+      <c r="B30">
+        <v>1.8889024109367936</v>
+      </c>
+      <c r="C30">
+        <v>218.71408566386901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>573</v>
+      </c>
+      <c r="B31">
+        <v>1.8210849869020718</v>
+      </c>
+      <c r="C31">
+        <v>261.61929580801097</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>573</v>
+      </c>
+      <c r="B32">
+        <v>2.2058574515399765</v>
+      </c>
+      <c r="C32">
+        <v>195.01569776964899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>573</v>
+      </c>
+      <c r="B33">
+        <v>3.0394617031643696</v>
+      </c>
+      <c r="C33">
+        <v>200.86212939797201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>573</v>
+      </c>
+      <c r="B34">
+        <v>2.8711550093042701</v>
+      </c>
+      <c r="C34">
+        <v>168.33189798011301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>573</v>
+      </c>
+      <c r="B35">
+        <v>2.7890092589565514</v>
+      </c>
+      <c r="C35">
+        <v>143.191233393224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>573</v>
+      </c>
+      <c r="B36">
+        <v>2.3182030649553669</v>
+      </c>
+      <c r="C36">
+        <v>129.91825348027399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>573</v>
+      </c>
+      <c r="B37">
+        <v>3.255508142141688</v>
+      </c>
+      <c r="C37">
+        <v>283.68377584060698</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>573</v>
+      </c>
+      <c r="B38">
+        <v>3.6185472227705286</v>
+      </c>
+      <c r="C38">
+        <v>344.30646423734299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>573</v>
+      </c>
+      <c r="B39">
+        <v>4.4067156707867881</v>
+      </c>
+      <c r="C39">
+        <v>313.18825195916003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>573</v>
+      </c>
+      <c r="B40">
+        <v>4.8285850751787507</v>
+      </c>
+      <c r="C40">
+        <v>339.78800299038198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>573</v>
+      </c>
+      <c r="B41">
+        <v>5.5573825832727115</v>
+      </c>
+      <c r="C41">
+        <v>319.03468358748398</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>573</v>
+      </c>
+      <c r="B42">
+        <v>7.5008047537216616</v>
+      </c>
+      <c r="C42">
+        <v>298.2208490786</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>573</v>
+      </c>
+      <c r="B43">
+        <v>7.1028366244252252</v>
+      </c>
+      <c r="C43">
+        <v>279.010664878348</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>573</v>
+      </c>
+      <c r="B44">
+        <v>6.3975391754033355</v>
+      </c>
+      <c r="C44">
+        <v>351.53129550201601</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>573</v>
+      </c>
+      <c r="B45">
+        <v>7.7715392604929203</v>
+      </c>
+      <c r="C45">
+        <v>326.31330605747797</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>573</v>
+      </c>
+      <c r="B46">
+        <v>8.9817211874328429</v>
+      </c>
+      <c r="C46">
+        <v>304.06728070692299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>573</v>
+      </c>
+      <c r="B47">
+        <v>8.8322349374210241</v>
+      </c>
+      <c r="C47">
+        <v>367.68210489963798</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>573</v>
+      </c>
+      <c r="B48">
+        <v>8.9030998329078344</v>
+      </c>
+      <c r="C48">
+        <v>423.890552509722</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>573</v>
+      </c>
+      <c r="B49">
+        <v>14.313688808668397</v>
+      </c>
+      <c r="C49">
+        <v>389.649088372591</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>573</v>
+      </c>
+      <c r="B50">
+        <v>14.686366589851643</v>
+      </c>
+      <c r="C50">
+        <v>425.137836083102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>573</v>
+      </c>
+      <c r="B51">
+        <v>15.648216603190019</v>
+      </c>
+      <c r="C51">
+        <v>349.66205111711201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>573</v>
+      </c>
+      <c r="B52">
+        <v>24.886066959035219</v>
+      </c>
+      <c r="C52">
+        <v>367.13074504509802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>573</v>
+      </c>
+      <c r="B53">
+        <v>26.885396749570141</v>
+      </c>
+      <c r="C53">
+        <v>399.62063305896601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>573</v>
+      </c>
+      <c r="B54">
+        <v>27.011217398783437</v>
+      </c>
+      <c r="C54">
+        <v>424.76465959618798</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>573</v>
+      </c>
+      <c r="B55">
+        <v>30.029790104167777</v>
+      </c>
+      <c r="C55">
+        <v>440.95917434813299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>573</v>
+      </c>
+      <c r="B56">
+        <v>68.821182944268017</v>
+      </c>
+      <c r="C56">
+        <v>450.54409474626402</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>573</v>
+      </c>
+      <c r="B57">
+        <v>86.105190734819658</v>
+      </c>
+      <c r="C57">
+        <v>494.65288310946198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>573</v>
+      </c>
+      <c r="B58">
+        <v>87.260604936417153</v>
+      </c>
+      <c r="C58">
+        <v>414.75613345615398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>623</v>
+      </c>
+      <c r="B59">
+        <v>0.8216719667627328</v>
+      </c>
+      <c r="C59">
+        <v>141.98764665450199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>623</v>
+      </c>
+      <c r="B60">
+        <v>0.73834593955070094</v>
+      </c>
+      <c r="C60">
+        <v>175.888150300825</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>623</v>
+      </c>
+      <c r="B61">
+        <v>2.3035558826092681</v>
+      </c>
+      <c r="C61">
+        <v>10.7884615848051</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>623</v>
+      </c>
+      <c r="B62">
+        <v>2.3863482541206378</v>
+      </c>
+      <c r="C62">
+        <v>171.182385576576</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>623</v>
+      </c>
+      <c r="B63">
+        <v>15.892301070449408</v>
+      </c>
+      <c r="C63">
+        <v>127.59052250088</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>623</v>
+      </c>
+      <c r="B64">
+        <v>35.071682091838326</v>
+      </c>
+      <c r="C64">
+        <v>-50.283789929195599</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>673</v>
+      </c>
+      <c r="B65">
+        <v>0.38104774779313821</v>
+      </c>
+      <c r="C65">
+        <v>61.353694094011203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>673</v>
+      </c>
+      <c r="B66">
+        <v>0.79481575717806974</v>
+      </c>
+      <c r="C66">
+        <v>63.722505201731202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>673</v>
+      </c>
+      <c r="B67">
+        <v>0.33286729215113525</v>
+      </c>
+      <c r="C67">
+        <v>21.042249733328699</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>673</v>
+      </c>
+      <c r="B68">
+        <v>0.57718758809855963</v>
+      </c>
+      <c r="C68">
+        <v>28.3236362801537</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>673</v>
+      </c>
+      <c r="B69">
+        <v>0.44692970898964179</v>
+      </c>
+      <c r="C69">
+        <v>-2.1987586611707002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>673</v>
+      </c>
+      <c r="B70">
+        <v>0.29894632789509701</v>
+      </c>
+      <c r="C70">
+        <v>-19.27197166265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>673</v>
+      </c>
+      <c r="B71">
+        <v>0.62585485525569762</v>
+      </c>
+      <c r="C71">
+        <v>-99.983725513495301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>673</v>
+      </c>
+      <c r="B72">
+        <v>0.67526763855784955</v>
+      </c>
+      <c r="C72">
+        <v>-123.208071696217</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>673</v>
+      </c>
+      <c r="B73">
+        <v>0.29971355930687404</v>
+      </c>
+      <c r="C73">
+        <v>-118.24550962177899</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>673</v>
+      </c>
+      <c r="B74">
+        <v>0.51888496624127312</v>
+      </c>
+      <c r="C74">
+        <v>-146.396316420087</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>673</v>
+      </c>
+      <c r="B75">
+        <v>0.85060482836623963</v>
+      </c>
+      <c r="C75">
+        <v>23.391621593974801</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>673</v>
+      </c>
+      <c r="B76">
+        <v>2.2225256660734893</v>
+      </c>
+      <c r="C76">
+        <v>63.558660119251201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>673</v>
+      </c>
+      <c r="B77">
+        <v>2.3481836707832264</v>
+      </c>
+      <c r="C77">
+        <v>-68.417165300773306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>673</v>
+      </c>
+      <c r="B78">
+        <v>9.0878366828936219</v>
+      </c>
+      <c r="C78">
+        <v>38.704194217617697</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>673</v>
+      </c>
+      <c r="B79">
+        <v>8.9069528289084321</v>
+      </c>
+      <c r="C79">
+        <v>-6.4976092997993096</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>673</v>
+      </c>
+      <c r="B80">
+        <v>9.9034264464485222</v>
+      </c>
+      <c r="C80">
+        <v>-6.5420418645396703</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>673</v>
+      </c>
+      <c r="B81">
+        <v>9.3997011469313154</v>
+      </c>
+      <c r="C81">
+        <v>-32.179631719721399</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>673</v>
+      </c>
+      <c r="B82">
+        <v>11.487617010676265</v>
+      </c>
+      <c r="C82">
+        <v>192.560280736968</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>673</v>
+      </c>
+      <c r="B83">
+        <v>15.039185046635005</v>
+      </c>
+      <c r="C83">
+        <v>31.136773035276999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>673</v>
+      </c>
+      <c r="B84">
+        <v>15.838562065075868</v>
+      </c>
+      <c r="C84">
+        <v>9.1148831358411808</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>673</v>
+      </c>
+      <c r="B85">
+        <v>16.003303634184427</v>
+      </c>
+      <c r="C85">
+        <v>-37.322701088416899</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>673</v>
+      </c>
+      <c r="B86">
+        <v>22.679412626529615</v>
+      </c>
+      <c r="C86">
+        <v>-47.306142978514202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>673</v>
+      </c>
+      <c r="B87">
+        <v>22.004894898342446</v>
+      </c>
+      <c r="C87">
+        <v>-11.8517333510115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>673</v>
+      </c>
+      <c r="B88">
+        <v>22.383797444261003</v>
+      </c>
+      <c r="C88">
+        <v>46.788143965064997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>673</v>
+      </c>
+      <c r="B89">
+        <v>21.337360726988532</v>
+      </c>
+      <c r="C89">
+        <v>72.478497490876407</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>673</v>
+      </c>
+      <c r="B90">
+        <v>31.184303444142678</v>
+      </c>
+      <c r="C90">
+        <v>58.7738283037746</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>673</v>
+      </c>
+      <c r="B91">
+        <v>33.377590462560697</v>
+      </c>
+      <c r="C91">
+        <v>51.389691450987797</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>673</v>
+      </c>
+      <c r="B92">
+        <v>38.376219208940498</v>
+      </c>
+      <c r="C92">
+        <v>-99.017317230392607</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>673</v>
+      </c>
+      <c r="B93">
+        <v>43.976720861312351</v>
+      </c>
+      <c r="C93">
+        <v>-80.808296792738005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>673</v>
+      </c>
+      <c r="B94">
+        <v>44.656939937944941</v>
+      </c>
+      <c r="C94">
+        <v>-123.588525531806</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>673</v>
+      </c>
+      <c r="B95">
+        <v>35.177412862657143</v>
+      </c>
+      <c r="C95">
+        <v>-140.489562344917</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>673</v>
+      </c>
+      <c r="B96">
+        <v>38.381367383433847</v>
+      </c>
+      <c r="C96">
+        <v>-157.668302687655</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>673</v>
+      </c>
+      <c r="B97">
+        <v>57.39851018296519</v>
+      </c>
+      <c r="C97">
+        <v>-87.176038727089804</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>673</v>
+      </c>
+      <c r="B98">
+        <v>58.630024437850146</v>
+      </c>
+      <c r="C98">
+        <v>-28.547269552197601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>723</v>
+      </c>
+      <c r="B99">
+        <v>8.7141183531620606E-2</v>
+      </c>
+      <c r="C99">
+        <v>-34.661256909477999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>723</v>
+      </c>
+      <c r="B100">
+        <v>5.4706175982531101E-2</v>
+      </c>
+      <c r="C100">
+        <v>38.477385846041201</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>723</v>
+      </c>
+      <c r="B101">
+        <v>8.7003610527051412E-2</v>
+      </c>
+      <c r="C101">
+        <v>-1.75634605832431</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>723</v>
+      </c>
+      <c r="B102">
+        <v>5.5286953029077841</v>
+      </c>
+      <c r="C102">
+        <v>28.148899939984599</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>723</v>
+      </c>
+      <c r="B103">
+        <v>5.0639389046408763</v>
+      </c>
+      <c r="C103">
+        <v>-15.6966167918139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>723</v>
+      </c>
+      <c r="B104">
+        <v>4.9286512261185678</v>
+      </c>
+      <c r="C104">
+        <v>-33.968813499310698</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>723</v>
+      </c>
+      <c r="B105">
+        <v>19.082316550739783</v>
+      </c>
+      <c r="C105">
+        <v>-108.896730026703</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>723</v>
+      </c>
+      <c r="B106">
+        <v>29.725895626594568</v>
+      </c>
+      <c r="C106">
+        <v>-82.381686964573404</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>723</v>
+      </c>
+      <c r="B107">
+        <v>32.094845564074369</v>
+      </c>
+      <c r="C107">
+        <v>-129.969167884916</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>723</v>
+      </c>
+      <c r="B108">
+        <v>31.9734231195843</v>
+      </c>
+      <c r="C108">
+        <v>-45.876070380549002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>723</v>
+      </c>
+      <c r="B109">
+        <v>33.949873937803311</v>
+      </c>
+      <c r="C109">
+        <v>-34.954852915389097</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>723</v>
+      </c>
+      <c r="B110">
+        <v>31.741871762376746</v>
+      </c>
+      <c r="C110">
+        <v>-10.528219178324701</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>723</v>
+      </c>
+      <c r="B111">
+        <v>29.720906157228121</v>
+      </c>
+      <c r="C111">
+        <v>-17.790565664160098</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>723</v>
+      </c>
+      <c r="B112">
+        <v>32.197879004999329</v>
+      </c>
+      <c r="C112">
+        <v>17.490810970688202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>723</v>
+      </c>
+      <c r="B113">
+        <v>35.258575726775391</v>
+      </c>
+      <c r="C113">
+        <v>-6.9552111818608804</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>773</v>
+      </c>
+      <c r="B114">
+        <v>7.7060423708193451E-2</v>
+      </c>
+      <c r="C114">
+        <v>-113.696221855674</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>773</v>
+      </c>
+      <c r="B115">
+        <v>4.2711656983129496</v>
+      </c>
+      <c r="C115">
+        <v>-69.767439227120093</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>773</v>
+      </c>
+      <c r="B116">
+        <v>4.3285566070817731</v>
+      </c>
+      <c r="C116">
+        <v>-18.5197812887894</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>773</v>
+      </c>
+      <c r="B117">
+        <v>44.282193640652828</v>
+      </c>
+      <c r="C117">
+        <v>-170.10786078180499</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>773</v>
+      </c>
+      <c r="B118">
+        <v>69.869661771176453</v>
+      </c>
+      <c r="C118">
+        <v>-189.366015443077</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>773</v>
+      </c>
+      <c r="B119">
+        <v>15.985614312160404</v>
+      </c>
+      <c r="C119">
+        <v>-85.670947592557397</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09146735-3AE3-45E3-9718-5F3A94A18F40}">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7.9055448E-2</v>
+      </c>
+      <c r="B3">
+        <v>47.419354269999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4.2852950000000001E-2</v>
+      </c>
+      <c r="B4">
+        <v>100.6928192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0.869426323</v>
+      </c>
+      <c r="B5">
+        <v>113.8077875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.98715820499999996</v>
+      </c>
+      <c r="B6">
+        <v>164.0857547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1.8889024109999999</v>
+      </c>
+      <c r="B7">
+        <v>218.7140857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1.8210849870000001</v>
+      </c>
+      <c r="B8">
+        <v>261.61929579999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2.2058574520000001</v>
+      </c>
+      <c r="B9">
+        <v>195.0156978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3.0394617030000002</v>
+      </c>
+      <c r="B10">
+        <v>200.86212939999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2.8711550090000002</v>
+      </c>
+      <c r="B11">
+        <v>168.331898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2.7890092590000002</v>
+      </c>
+      <c r="B12">
+        <v>143.19123339999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2.3182030650000001</v>
+      </c>
+      <c r="B13">
+        <v>129.91825349999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3.255508142</v>
+      </c>
+      <c r="B14">
+        <v>283.68377579999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3.6185472230000002</v>
+      </c>
+      <c r="B15">
+        <v>344.30646419999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4.4067156709999997</v>
+      </c>
+      <c r="B16">
+        <v>313.18825199999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>4.8285850750000003</v>
+      </c>
+      <c r="B17">
+        <v>339.788003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5.5573825829999999</v>
+      </c>
+      <c r="B18">
+        <v>319.03468359999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>7.5008047539999998</v>
+      </c>
+      <c r="B19">
+        <v>298.22084910000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>7.102836624</v>
+      </c>
+      <c r="B20">
+        <v>279.01066489999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>6.3975391750000004</v>
+      </c>
+      <c r="B21">
+        <v>351.5312955</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>7.7715392599999999</v>
+      </c>
+      <c r="B22">
+        <v>326.31330609999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>8.9817211869999998</v>
+      </c>
+      <c r="B23">
+        <v>304.06728070000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>8.8322349370000008</v>
+      </c>
+      <c r="B24">
+        <v>367.68210490000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>8.9030998330000006</v>
+      </c>
+      <c r="B25">
+        <v>423.89055250000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>14.31368881</v>
+      </c>
+      <c r="B26">
+        <v>389.64908839999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>14.68636659</v>
+      </c>
+      <c r="B27">
+        <v>425.13783610000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>15.6482166</v>
+      </c>
+      <c r="B28">
+        <v>349.66205109999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>24.886066960000001</v>
+      </c>
+      <c r="B29">
+        <v>367.13074499999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>26.885396750000002</v>
+      </c>
+      <c r="B30">
+        <v>399.62063310000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>27.0112174</v>
+      </c>
+      <c r="B31">
+        <v>424.76465960000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30.0297901</v>
+      </c>
+      <c r="B32">
+        <v>440.95917429999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>68.82118294</v>
+      </c>
+      <c r="B33">
+        <v>450.54409470000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>86.105190730000004</v>
+      </c>
+      <c r="B34">
+        <v>494.6528831</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>87.260604939999993</v>
+      </c>
+      <c r="B35">
+        <v>414.75613349999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D9E279-F5C1-4A33-B324-EEBF802E59BB}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>535.90126750000002</v>
+      </c>
+      <c r="B3">
+        <v>40.628102609999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>559.82328050000001</v>
+      </c>
+      <c r="B4">
+        <v>149.84685569999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>568.71572079999999</v>
+      </c>
+      <c r="B5">
+        <v>318.52328949999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>929.69532200000003</v>
+      </c>
+      <c r="B6">
+        <v>337.8366292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1042.9778590000001</v>
+      </c>
+      <c r="B7">
+        <v>339.72892469999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1411.8006190000001</v>
+      </c>
+      <c r="B8">
+        <v>243.56611079999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1181.4418310000001</v>
+      </c>
+      <c r="B9">
+        <v>351.13557420000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1282.559947</v>
+      </c>
+      <c r="B10">
+        <v>362.62322560000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1436.9150340000001</v>
+      </c>
+      <c r="B11">
+        <v>395.24788569999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1675.5668209999999</v>
+      </c>
+      <c r="B12">
+        <v>401.2285296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1258.6891889999999</v>
+      </c>
+      <c r="B13">
+        <v>408.2891995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1335.2461350000001</v>
+      </c>
+      <c r="B14">
+        <v>478.1803812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1342.697345</v>
+      </c>
+      <c r="B15">
+        <v>472.86237829999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1794.483757</v>
+      </c>
+      <c r="B16">
+        <v>596.27222280000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added F82H radiation sections 5.2 Ductility and 5.3 Stress-Strain Relationship
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDBA03-8FFF-4596-9150-9C1DA2CD6DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B5E06-B3C8-4540-96B7-5B1782B09C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17330" yWindow="4040" windowWidth="18500" windowHeight="16010" tabRatio="736" firstSheet="13" activeTab="14" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="17710" yWindow="3620" windowWidth="18500" windowHeight="16010" tabRatio="736" firstSheet="13" activeTab="15" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Radiation Hardening 3D" sheetId="19" r:id="rId13"/>
     <sheet name="Radiation Hardening - No Helium" sheetId="20" r:id="rId14"/>
     <sheet name="Helium Hardening" sheetId="21" r:id="rId15"/>
+    <sheet name="Radiation Elongation" sheetId="22" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>F82H</t>
   </si>
@@ -365,6 +366,9 @@
   </si>
   <si>
     <t>He conc (appm)</t>
+  </si>
+  <si>
+    <t>elongation</t>
   </si>
 </sst>
 </file>
@@ -2631,7 +2635,7 @@
   <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4258,7 +4262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D9E279-F5C1-4A33-B324-EEBF802E59BB}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -4397,6 +4401,1125 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECDC948-454D-43CF-A165-3099DA1EB130}">
+  <dimension ref="A1:C100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>290.59538000466728</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>11.8408860809863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>525.22133779675403</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>8.4786989052001402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>522.17009426160894</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>7.2652661641914298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>622.75275037924598</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>7.1427636764762399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>672.61637021691195</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6.7998435683779404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>721.24484935510895</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>10.9196954350233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>722.31958929077598</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>8.5800215245729898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>772.20336847014198</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>13.9131725052974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>773.232279616151</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>12.180098041788099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>820.95296655243396</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>16.429868690741699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>920.63162238497898</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>22.329998733779199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>922.16189516409099</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>19.903701166212599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>289.63869375836299</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>23.6550589869214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>574.64172011863798</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>15.6395117708611</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>575.24476560195399</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>7.6574756011297103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>575.90629151628195</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>6.4000736992534799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>672.72086627751196</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>14.717388941312199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>673.51456654434799</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>11.7104996597688</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>771.98741361580801</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>20.574656164752</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>771.12349572420294</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>24.510960616743599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>290.51606141127172</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>18.656907852154902</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>350.9099685369012</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>15.1384264831902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>470.76560138196101</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>13.3340483850239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>574.58995614759999</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>10.544116828608001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>672.34842813577097</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>9.87788061371125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>722.80104459532299</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>10.0370599000212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>774.217775344968</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>11.646947673208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>822.421205055511</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>13.152979450308001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>291.01023341269439</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>15.1365483459365</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>673.28465564575299</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>8.6325003580388895</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>870.74020947072995</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>25.6839287061396</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>971.05019154393096</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>24.019074544251701</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>289.9849938662968</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>21.169446945746198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>292.08334122670442</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>19.959147219088699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>293.8665218523642</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>16.279494100526499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>770.61134700626803</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>21.544135522793901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>602.87333242359102</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>17.176710265882399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>604.45797532343204</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>15.3978453590444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>617.60174404913596</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>13.8941373526247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>603.28706406319304</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>13.4612407360221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>645.096421450766</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>13.811463482084299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>688.47593026218703</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>11.987566313598</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>649.419228739495</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>11.716032282178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>691.19090828948697</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>11.0385920081925</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>691.67564816145398</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>9.2598720161145103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>663.044839041969</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>8.3545532821381698</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>674.10183522467196</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>9.9341241653815509</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>731.45040231960195</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>14.1162916795983</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>729.83242902497705</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>14.9860700687017</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>739.22073174707998</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>16.052026814061101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>739.33666355502498</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>19.2140668757465</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>764.08882912496904</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>19.329382795961202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>764.11056633895805</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>19.922265307527201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>778.38322104452197</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>19.208922401768898</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>777.37896175820299</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>21.817750367419301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>777.40939385778802</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>22.6477858836117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>798.89807903409496</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>23.751674067382901</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>776.55222305279904</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>14.268452177525401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>835.57672934632603</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>19.1618613334815</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>834.99344743760503</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>18.2528472731269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>895.15408544898798</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>24.134249033599701</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>894.08026707790304</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>24.845852962238801</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>872.1662570812</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>27.1412303021594</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>904.21922825644594</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>16.386019107011101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>560.75385744976597</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>8.3680303548117099</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>629.607931909385</v>
+      </c>
+      <c r="B68">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>11.3629112409172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>629.66010122295995</v>
+      </c>
+      <c r="B69">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>12.785829268675601</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>648.330918892417</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>12.0323812031065</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>647.11073661380101</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>8.75190955386784</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>672.50994658683499</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>11.515361568364099</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>732.511178362294</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="C73">
+        <v>13.0489582440195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>732.92925744469403</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>9.4520652164724606</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>731.50836822357496</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75">
+        <v>15.697311710440999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>821.14177010963999</v>
+      </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>15.4483481528802</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>906.02993818177902</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+      <c r="C77">
+        <v>20.773132320459698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>557.999752437285</v>
+      </c>
+      <c r="B78">
+        <v>30</v>
+      </c>
+      <c r="C78">
+        <v>8.2498161393983303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>628.56309649028503</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="C79">
+        <v>12.8650251849777</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>671.96724081089496</v>
+      </c>
+      <c r="B80">
+        <v>30</v>
+      </c>
+      <c r="C80">
+        <v>11.713061529599401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>732.60537295624897</v>
+      </c>
+      <c r="B81">
+        <v>30</v>
+      </c>
+      <c r="C81">
+        <v>15.6181157941389</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>735.81088744591398</v>
+      </c>
+      <c r="B82">
+        <v>30</v>
+      </c>
+      <c r="C82">
+        <v>13.048523499739799</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>734.07988063854305</v>
+      </c>
+      <c r="B83">
+        <v>30</v>
+      </c>
+      <c r="C83">
+        <v>10.8353128286999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>758.72625843373703</v>
+      </c>
+      <c r="B84">
+        <v>30</v>
+      </c>
+      <c r="C84">
+        <v>8.0652671926267399</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>783.48856803687602</v>
+      </c>
+      <c r="B85">
+        <v>30</v>
+      </c>
+      <c r="C85">
+        <v>8.4572616182389702</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>782.34374143342495</v>
+      </c>
+      <c r="B86">
+        <v>30</v>
+      </c>
+      <c r="C86">
+        <v>7.2321160090958099</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>820.53095439653305</v>
+      </c>
+      <c r="B87">
+        <v>30</v>
+      </c>
+      <c r="C87">
+        <v>13.788349577875399</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>816.06902893826998</v>
+      </c>
+      <c r="B88">
+        <v>30</v>
+      </c>
+      <c r="C88">
+        <v>12.089332703759201</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>903.83737786402901</v>
+      </c>
+      <c r="B89">
+        <v>30</v>
+      </c>
+      <c r="C89">
+        <v>20.9710496538349</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>835.82091071680895</v>
+      </c>
+      <c r="B90">
+        <v>30</v>
+      </c>
+      <c r="C90">
+        <v>10.821908213406299</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>836.314345474373</v>
+      </c>
+      <c r="B91">
+        <v>30</v>
+      </c>
+      <c r="C91">
+        <v>9.2803412259547091</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>670.79053296025904</v>
+      </c>
+      <c r="B92">
+        <v>50</v>
+      </c>
+      <c r="C92">
+        <v>9.6183549034928095</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>646.50137004829298</v>
+      </c>
+      <c r="B93">
+        <v>50</v>
+      </c>
+      <c r="C93">
+        <v>7.1314364796340399</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>667.36040059270204</v>
+      </c>
+      <c r="B94">
+        <v>50</v>
+      </c>
+      <c r="C94">
+        <v>6.0614945783765402</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>667.79297115109398</v>
+      </c>
+      <c r="B95">
+        <v>50</v>
+      </c>
+      <c r="C95">
+        <v>2.8598565585401299</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>703.20434188773197</v>
+      </c>
+      <c r="B96">
+        <v>50</v>
+      </c>
+      <c r="C96">
+        <v>8.7049934003402996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>741.08868300258598</v>
+      </c>
+      <c r="B97">
+        <v>50</v>
+      </c>
+      <c r="C97">
+        <v>7.0003973079668098</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>718.52617945519296</v>
+      </c>
+      <c r="B98">
+        <v>50</v>
+      </c>
+      <c r="C98">
+        <v>6.6081130528347103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>903.17729113254495</v>
+      </c>
+      <c r="B99">
+        <v>50</v>
+      </c>
+      <c r="C99">
+        <v>17.9671840526137</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>291.6870057970591</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>15.220611791283099</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added F82H irradiated sections 5.4 and most of 5.5
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B5E06-B3C8-4540-96B7-5B1782B09C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8AB393-1B35-4561-A11C-AAF704CDC168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17710" yWindow="3620" windowWidth="18500" windowHeight="16010" tabRatio="736" firstSheet="13" activeTab="15" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="14150" yWindow="0" windowWidth="24340" windowHeight="20970" tabRatio="585" firstSheet="15" activeTab="17" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -29,6 +29,8 @@
     <sheet name="Radiation Hardening - No Helium" sheetId="20" r:id="rId14"/>
     <sheet name="Helium Hardening" sheetId="21" r:id="rId15"/>
     <sheet name="Radiation Elongation" sheetId="22" r:id="rId16"/>
+    <sheet name="Swelling Rate Temp Dependence" sheetId="23" r:id="rId17"/>
+    <sheet name="Swelling Rate Dose Dependence" sheetId="24" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>F82H</t>
   </si>
@@ -369,6 +371,15 @@
   </si>
   <si>
     <t>elongation</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>HT9</t>
+  </si>
+  <si>
+    <t>Volumetric Swelling (%)</t>
   </si>
 </sst>
 </file>
@@ -4410,8 +4421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECDC948-454D-43CF-A165-3099DA1EB130}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5520,6 +5531,400 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CFE494-FC8E-453E-80BE-48D9BDDA2137}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>484.95290119999999</v>
+      </c>
+      <c r="B3">
+        <v>3.3850829999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>530.4025762</v>
+      </c>
+      <c r="B4">
+        <v>0.107457315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>571.5197177</v>
+      </c>
+      <c r="B5">
+        <v>0.267528127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>598.50022130000002</v>
+      </c>
+      <c r="B6">
+        <v>0.43391721599999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>623.20614469999998</v>
+      </c>
+      <c r="B7">
+        <v>0.59570007700000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>652.50315620000003</v>
+      </c>
+      <c r="B8">
+        <v>0.78521348199999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>681.64643260000003</v>
+      </c>
+      <c r="B9">
+        <v>0.90682723399999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>728.1722532</v>
+      </c>
+      <c r="B10">
+        <v>0.95573129000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>759.33155529999999</v>
+      </c>
+      <c r="B11">
+        <v>0.96775639999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>798.38026130000003</v>
+      </c>
+      <c r="B12">
+        <v>0.964268244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>822.61799169999995</v>
+      </c>
+      <c r="B13">
+        <v>0.91926579900000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>841.04872939999996</v>
+      </c>
+      <c r="B14">
+        <v>0.80950828100000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>851.02403860000004</v>
+      </c>
+      <c r="B15">
+        <v>0.71526985200000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>861.3697095</v>
+      </c>
+      <c r="B16">
+        <v>0.53460785899999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>865.49609840000005</v>
+      </c>
+      <c r="B17">
+        <v>0.35709627100000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>872.42116420000002</v>
+      </c>
+      <c r="B18">
+        <v>0.16566700100000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>875.51682930000004</v>
+      </c>
+      <c r="B19">
+        <v>3.2919102999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EC7B2A-221C-4D3B-ADBB-F996565690DA}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>71.609244905872501</v>
+      </c>
+      <c r="B4">
+        <v>0.15950939557271199</v>
+      </c>
+      <c r="C4">
+        <v>126.375854386866</v>
+      </c>
+      <c r="D4">
+        <v>9.3519322700324203E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>130.577498987685</v>
+      </c>
+      <c r="B5">
+        <v>0.40667169366411998</v>
+      </c>
+      <c r="C5">
+        <v>249.93825950467399</v>
+      </c>
+      <c r="D5">
+        <v>0.33015068114861501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>197.929010592465</v>
+      </c>
+      <c r="B6">
+        <v>1.8507554089109499</v>
+      </c>
+      <c r="C6">
+        <v>348.22168772616101</v>
+      </c>
+      <c r="D6">
+        <v>0.65649534335012305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>247.71975109208401</v>
+      </c>
+      <c r="B7">
+        <v>3.5259474626301901</v>
+      </c>
+      <c r="C7">
+        <v>452.10296855169599</v>
+      </c>
+      <c r="D7">
+        <v>1.5240101131360599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>346.62716610411002</v>
+      </c>
+      <c r="B8">
+        <v>6.0775826914849604</v>
+      </c>
+      <c r="C8">
+        <v>551.08550235872997</v>
+      </c>
+      <c r="D8">
+        <v>1.9358328098864901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>449.041126467141</v>
+      </c>
+      <c r="B9">
+        <v>8.7427689217090503</v>
+      </c>
+      <c r="C9">
+        <v>651.44521407425805</v>
+      </c>
+      <c r="D9">
+        <v>3.1177590847239798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>545.77810909538402</v>
+      </c>
+      <c r="B10">
+        <v>13.1207209114986</v>
+      </c>
+      <c r="C10">
+        <v>35.789512203394096</v>
+      </c>
+      <c r="D10">
+        <v>0.20332891239581899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>650.29439413472505</v>
+      </c>
+      <c r="B11">
+        <v>15.8996870765625</v>
+      </c>
+      <c r="C11">
+        <v>33.628280671815901</v>
+      </c>
+      <c r="D11">
+        <v>0.87446114245831397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>183.360168364533</v>
+      </c>
+      <c r="D12">
+        <v>1.5978797350293501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>202.497085929816</v>
+      </c>
+      <c r="D13">
+        <v>1.76489121102152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>207.41039568878301</v>
+      </c>
+      <c r="D14">
+        <v>1.91362838777394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>207.791054473923</v>
+      </c>
+      <c r="D15">
+        <v>1.99922083207637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>207.65137545897699</v>
+      </c>
+      <c r="D16">
+        <v>2.5217408378598898</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>207.68707616567301</v>
+      </c>
+      <c r="D17">
+        <v>2.6118315712059501</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated missing links in Eurofer and F82H
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Repos\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8AB393-1B35-4561-A11C-AAF704CDC168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCFA9C1-91C6-413B-BC8C-BFF146DE3E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14150" yWindow="0" windowWidth="24340" windowHeight="20970" tabRatio="585" firstSheet="15" activeTab="17" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="585" firstSheet="1" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -2346,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA6CA63-0F6B-4003-854E-C3B2C624AC7C}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2506,6 +2506,14 @@
       </c>
       <c r="B19">
         <v>333.05233620000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5711,7 +5719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EC7B2A-221C-4D3B-ADBB-F996565690DA}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reorganized the table of contents for F82H
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Repos\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCFA9C1-91C6-413B-BC8C-BFF146DE3E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999507C-0EE3-4822-8EC7-D00FEEFA3195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="585" firstSheet="1" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
@@ -2349,7 +2349,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed F82H ToC links
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Repos\DatabaseCodes\Jupyter\F82H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999507C-0EE3-4822-8EC7-D00FEEFA3195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E639D6-371A-4AF8-BB5C-DE8D71099AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="585" firstSheet="1" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="5630" yWindow="3960" windowWidth="18500" windowHeight="16010" tabRatio="585" firstSheet="17" activeTab="18" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="Radiation Elongation" sheetId="22" r:id="rId16"/>
     <sheet name="Swelling Rate Temp Dependence" sheetId="23" r:id="rId17"/>
     <sheet name="Swelling Rate Dose Dependence" sheetId="24" r:id="rId18"/>
+    <sheet name="Radiation Toughness" sheetId="25" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
   <si>
     <t>F82H</t>
   </si>
@@ -380,6 +381,15 @@
   </si>
   <si>
     <t>Volumetric Swelling (%)</t>
+  </si>
+  <si>
+    <t>K_4 [MPa m^(1/2)]</t>
+  </si>
+  <si>
+    <t>T (C)</t>
+  </si>
+  <si>
+    <t>K_un [MPa m^(1/2)]</t>
   </si>
 </sst>
 </file>
@@ -2348,8 +2358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA6CA63-0F6B-4003-854E-C3B2C624AC7C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5933,6 +5943,184 @@
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F95D61-C37C-4912-95F8-DA471543138A}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>-80.392004198603104</v>
+      </c>
+      <c r="B3">
+        <v>38.017544163191801</v>
+      </c>
+      <c r="C3">
+        <v>-10.058336361172101</v>
+      </c>
+      <c r="D3">
+        <v>31.093309341315301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>-82.002814448270101</v>
+      </c>
+      <c r="B4">
+        <v>61.100057096389001</v>
+      </c>
+      <c r="C4">
+        <v>-10.1461436868119</v>
+      </c>
+      <c r="D4">
+        <v>48.704950083914397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-50.1206810042043</v>
+      </c>
+      <c r="B5">
+        <v>66.455006315206603</v>
+      </c>
+      <c r="C5">
+        <v>23.833272776557099</v>
+      </c>
+      <c r="D5">
+        <v>33.404848002491498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-41.632639525696199</v>
+      </c>
+      <c r="B6">
+        <v>63.996401197293999</v>
+      </c>
+      <c r="C6">
+        <v>70.609345352411694</v>
+      </c>
+      <c r="D6">
+        <v>51.461148502517403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>-41.7053076572601</v>
+      </c>
+      <c r="B7">
+        <v>78.571552156686394</v>
+      </c>
+      <c r="C7">
+        <v>120.802838670981</v>
+      </c>
+      <c r="D7">
+        <v>84.080488606675104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-50.269045106147303</v>
+      </c>
+      <c r="B8">
+        <v>96.212606190632698</v>
+      </c>
+      <c r="C8">
+        <v>119.261668714062</v>
+      </c>
+      <c r="D8">
+        <v>93.195148537121298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>-60.7726179559493</v>
+      </c>
+      <c r="B9">
+        <v>102.92921777946999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>-40.889809736376201</v>
+      </c>
+      <c r="B10">
+        <v>115.00596916795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-30.981711853556401</v>
+      </c>
+      <c r="B11">
+        <v>127.724622385245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-62.018068988586499</v>
+      </c>
+      <c r="B12">
+        <v>152.73111061127699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>-50.100495412103299</v>
+      </c>
+      <c r="B13">
+        <v>162.40635327093099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>-32.287719662496897</v>
+      </c>
+      <c r="B14">
+        <v>189.67247434987999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6808,7 +6996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41CB5B8-2BC3-43D2-A2E9-D01F45547500}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added F82H section 5.6 Irradiated Creep
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/F82H_data.xlsx
+++ b/Jupyter/F82H/F82H_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indro\Documents\GitHub\DatabaseCodes\Jupyter\F82H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E639D6-371A-4AF8-BB5C-DE8D71099AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75057D34-F187-4DAF-B0ED-3B4B6452E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5630" yWindow="3960" windowWidth="18500" windowHeight="16010" tabRatio="585" firstSheet="17" activeTab="18" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="15900" yWindow="4660" windowWidth="18500" windowHeight="16010" tabRatio="585" firstSheet="17" activeTab="19" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Swelling Rate Temp Dependence" sheetId="23" r:id="rId17"/>
     <sheet name="Swelling Rate Dose Dependence" sheetId="24" r:id="rId18"/>
     <sheet name="Radiation Toughness" sheetId="25" r:id="rId19"/>
+    <sheet name="Radiation Creep" sheetId="26" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t>F82H</t>
   </si>
@@ -390,6 +391,24 @@
   </si>
   <si>
     <t>K_un [MPa m^(1/2)]</t>
+  </si>
+  <si>
+    <t>Stress_573K (MPa)</t>
+  </si>
+  <si>
+    <t>Strain per dose_573K (%/dpa)</t>
+  </si>
+  <si>
+    <t>Stress_673K (MPa)</t>
+  </si>
+  <si>
+    <t>Strain per dose_673K (%/dpa)</t>
+  </si>
+  <si>
+    <t>Stress_773K (MPa)</t>
+  </si>
+  <si>
+    <t>Strain per dose_773K (%/dpa)</t>
   </si>
 </sst>
 </file>
@@ -4440,7 +4459,7 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5952,8 +5971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F95D61-C37C-4912-95F8-DA471543138A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6237,6 +6256,232 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E23EDCA-4B4C-46A6-8121-8BB4D5058F06}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>136.25551958535101</v>
+      </c>
+      <c r="B4">
+        <v>2.4820190358763101E-2</v>
+      </c>
+      <c r="C4">
+        <v>84.480490732837097</v>
+      </c>
+      <c r="D4">
+        <v>2.13919404499501E-2</v>
+      </c>
+      <c r="E4">
+        <v>49.724942975982898</v>
+      </c>
+      <c r="F4">
+        <v>1.2439316687605799E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>213.48000027076901</v>
+      </c>
+      <c r="B5">
+        <v>3.11437190245142E-2</v>
+      </c>
+      <c r="C5">
+        <v>126.931783984097</v>
+      </c>
+      <c r="D5">
+        <v>1.5585393139611201E-2</v>
+      </c>
+      <c r="E5">
+        <v>77.672200334215702</v>
+      </c>
+      <c r="F5">
+        <v>2.5526481099740098E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>282.785647899129</v>
+      </c>
+      <c r="B6">
+        <v>3.6361125748105697E-2</v>
+      </c>
+      <c r="C6">
+        <v>146.33071716151599</v>
+      </c>
+      <c r="D6">
+        <v>3.6422637079099297E-2</v>
+      </c>
+      <c r="E6">
+        <v>135.57932742153901</v>
+      </c>
+      <c r="F6">
+        <v>0.18552779234719399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>343.16917726212199</v>
+      </c>
+      <c r="B7">
+        <v>4.4112474903454602E-2</v>
+      </c>
+      <c r="C7">
+        <v>170.09607826002801</v>
+      </c>
+      <c r="D7">
+        <v>3.9855361220351701E-2</v>
+      </c>
+      <c r="E7">
+        <v>170.045009331203</v>
+      </c>
+      <c r="F7">
+        <v>0.289900650134784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>85.269805011147696</v>
+      </c>
+      <c r="B8">
+        <v>5.16261171247147E-3</v>
+      </c>
+      <c r="C8">
+        <v>216.06575424520301</v>
+      </c>
+      <c r="D8">
+        <v>8.2220543722155606E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>128.136088623429</v>
+      </c>
+      <c r="B9">
+        <v>9.53676128399919E-3</v>
+      </c>
+      <c r="C9">
+        <v>212.866493728644</v>
+      </c>
+      <c r="D9">
+        <v>5.9602053212086198E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>214.11871644884599</v>
+      </c>
+      <c r="B10">
+        <v>2.6272326338628901E-2</v>
+      </c>
+      <c r="C10">
+        <v>102.574924069624</v>
+      </c>
+      <c r="D10">
+        <v>2.0079010282619499E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>258.07369184738701</v>
+      </c>
+      <c r="B11">
+        <v>3.7713622547510199E-2</v>
+      </c>
+      <c r="C11">
+        <v>207.09171413585801</v>
+      </c>
+      <c r="D11">
+        <v>1.8199504775380099E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>291.96181711800898</v>
+      </c>
+      <c r="B12">
+        <v>6.1117902528849799E-2</v>
+      </c>
+      <c r="C12">
+        <v>208.735957454594</v>
+      </c>
+      <c r="D12">
+        <v>8.0653306173230896E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>